<commit_message>
revisi - 8 validasi, chart
</commit_message>
<xml_diff>
--- a/public/assets/file/data-alumni/Format.xlsx
+++ b/public/assets/file/data-alumni/Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dava\Documents\XI RPL1 Dava Ardiansyah\file penting\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bkk\public\assets\file\data-alumni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811014DA-7757-4237-A06A-262FCE4C5B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349A58EF-8C40-4E3E-A211-FD4AB03C7280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FC3AF8D6-8358-483C-8077-ED3F7D8E12D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nik</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>tahun_lulus</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
@@ -404,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52350605-DAB8-4E36-9267-22A2CADE6DE8}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +417,7 @@
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,9 +433,6 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>